<commit_message>
updated formula quick ratio
</commit_message>
<xml_diff>
--- a/Valuation_Engine_Mapping.xlsx
+++ b/Valuation_Engine_Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\GitHub\hellotaoworld\valuation_engine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tao_project\valuation_engine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888C9F9B-2E23-40D9-BB11-C06166D49C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2B4D29-1B53-46BE-BF8C-E9DA98F481A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="722" activeTab="3" xr2:uid="{DB505F9D-00EE-40BB-9331-63CC137490AC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="722" activeTab="3" xr2:uid="{DB505F9D-00EE-40BB-9331-63CC137490AC}"/>
   </bookViews>
   <sheets>
     <sheet name="BS tags" sheetId="16" r:id="rId1"/>
@@ -21,10 +21,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Formula!$A$1:$E$35</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -997,7 +1006,7 @@
     <t>RevenueFromContractWithCustomerIncludingAssessedTax</t>
   </si>
   <si>
-    <t>(q_df.loc[index,'bs.cash_n_equivalent']+ ad(q_df,index,'bs.st_investment')+ad(q_df.loc[index,'bs.account_receivable']))/q_df.loc[index,'bs.total_current_liabilities']</t>
+    <t>(q_df.loc[index,'bs.cash_n_equivalent']+ ad(q_df,index,'bs.st_investment')+ad(q_df,index,'bs.account_receivable'))/q_df.loc[index,'bs.total_current_liabilities']</t>
   </si>
 </sst>
 </file>
@@ -1005,7 +1014,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -1060,18 +1069,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2085,9 +2094,9 @@
   </sheetPr>
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B14" sqref="B14"/>
+      <selection pane="topRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add formula mapping step
</commit_message>
<xml_diff>
--- a/Valuation_Engine_Mapping.xlsx
+++ b/Valuation_Engine_Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tao_project\valuation_engine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81301F85-7B37-4019-80E8-A882F81C4E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9656DBFC-6F6D-4045-848E-9A7A1958485D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="722" activeTab="3" xr2:uid="{DB505F9D-00EE-40BB-9331-63CC137490AC}"/>
   </bookViews>
@@ -988,9 +988,6 @@
     <t>PayablesToTradeBrokersDealersAndClearingOrganizations</t>
   </si>
   <si>
-    <t>Valuation Ratio</t>
-  </si>
-  <si>
     <t>price_earnings_ratio</t>
   </si>
   <si>
@@ -1007,6 +1004,9 @@
   </si>
   <si>
     <t>(q_df.loc[index, 'bs.cash_n_equivalent'] + ad(q_df,index,'bs.st_investment') +ad(q_df,index,'bs.account_receivable'))/q_df.loc[index, 'bs.total_current_liabilities']</t>
+  </si>
+  <si>
+    <t>Custom Ratio</t>
   </si>
 </sst>
 </file>
@@ -2075,7 +2075,7 @@
     </row>
     <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>302</v>
@@ -2094,9 +2094,9 @@
   </sheetPr>
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2391,7 +2391,7 @@
         <v>134</v>
       </c>
       <c r="B13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C13" t="s">
         <v>50</v>
@@ -2918,19 +2918,19 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B36" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C36" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D36" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E36" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="F36" t="s">
         <v>160</v>

</xml_diff>

<commit_message>
add new run trigger
</commit_message>
<xml_diff>
--- a/Valuation_Engine_Mapping.xlsx
+++ b/Valuation_Engine_Mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\GitHub\hellotaoworld\valuation_engine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tao_project\valuation_engine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84DD6CE-44B9-4BA0-AC88-7DB49305F18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE038BE-6E55-4131-A666-D109C6532A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="722" activeTab="2" xr2:uid="{DB505F9D-00EE-40BB-9331-63CC137490AC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="722" activeTab="3" xr2:uid="{DB505F9D-00EE-40BB-9331-63CC137490AC}"/>
   </bookViews>
   <sheets>
     <sheet name="BS tags" sheetId="16" r:id="rId1"/>
@@ -21,10 +21,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Formula!$A$1:$E$35</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -194,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="325">
   <si>
     <t>is.net_revenue</t>
   </si>
@@ -1123,9 +1132,6 @@
     <t>PayablesToTradeBrokersDealersAndClearingOrganizations</t>
   </si>
   <si>
-    <t>price_earnings_ratio</t>
-  </si>
-  <si>
     <t>Stock_Price/curr_eps</t>
   </si>
   <si>
@@ -1169,6 +1175,9 @@
   </si>
   <si>
     <t>ProfitLoss</t>
+  </si>
+  <si>
+    <t>pe_ratio</t>
   </si>
 </sst>
 </file>
@@ -1176,7 +1185,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1244,18 +1253,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1812,7 +1821,7 @@
         <v>211</v>
       </c>
       <c r="N4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="O4" s="6" t="s">
         <v>301</v>
@@ -2009,7 +2018,7 @@
   </sheetPr>
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
@@ -2184,7 +2193,7 @@
         <v>267</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>275</v>
@@ -2252,12 +2261,12 @@
         <v>280</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>296</v>
@@ -2276,9 +2285,9 @@
   </sheetPr>
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2435,7 +2444,7 @@
         <v>126</v>
       </c>
       <c r="B7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C7" t="s">
         <v>216</v>
@@ -2504,7 +2513,7 @@
         <v>129</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C10" t="s">
         <v>45</v>
@@ -2573,7 +2582,7 @@
         <v>132</v>
       </c>
       <c r="B13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C13" t="s">
         <v>50</v>
@@ -2734,7 +2743,7 @@
         <v>140</v>
       </c>
       <c r="B20" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C20" t="s">
         <v>57</v>
@@ -2873,7 +2882,7 @@
         <v>146</v>
       </c>
       <c r="B26" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C26" t="s">
         <v>63</v>
@@ -2896,7 +2905,7 @@
         <v>147</v>
       </c>
       <c r="B27" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C27" t="s">
         <v>64</v>
@@ -2919,7 +2928,7 @@
         <v>148</v>
       </c>
       <c r="B28" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C28" t="s">
         <v>65</v>
@@ -3100,19 +3109,19 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B36" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C36" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D36" t="s">
-        <v>309</v>
+        <v>324</v>
       </c>
       <c r="E36" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F36" t="s">
         <v>158</v>

</xml_diff>